<commit_message>
Uppdatering av Jiro f�r veckan, 25/1
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering.xlsx
+++ b/Grafik/Planering/Grafikplanering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
   <si>
     <t>Vecka:</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>6.3 Menybakgrund</t>
-  </si>
-  <si>
-    <t>50% Färdigt</t>
   </si>
   <si>
     <t>73% Färdigt</t>
@@ -285,7 +282,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +307,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -350,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,11 +355,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -419,37 +404,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="6" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="7" builtinId="33"/>
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="6" builtinId="33"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O103"/>
+  <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,19 +1212,15 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>2</v>
-      </c>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="6"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1250,15 +1228,19 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="6"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1267,18 +1249,14 @@
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="6"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1288,7 +1266,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1308,7 +1286,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1328,16 +1306,16 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="6"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="9" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1347,14 +1325,18 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="6"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1362,36 +1344,36 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
-        <v>3</v>
-      </c>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1399,17 +1381,13 @@
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1419,17 +1397,17 @@
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="6"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1441,15 +1419,15 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1461,7 +1439,7 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="6"/>
@@ -1481,15 +1459,15 @@
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="9"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1501,15 +1479,15 @@
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="9"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1521,7 +1499,7 @@
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="6"/>
@@ -1541,17 +1519,17 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="6"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1561,7 +1539,7 @@
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="6"/>
@@ -1581,17 +1559,17 @@
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="6"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -1619,20 +1597,18 @@
       <c r="N43" s="1"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="3"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="C44" s="3"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="E44" s="1"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="G44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -1641,14 +1617,20 @@
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="E45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -1657,19 +1639,15 @@
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -1677,15 +1655,19 @@
       <c r="N46" s="1"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -1693,17 +1675,13 @@
       <c r="N47" s="1"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="6"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -1713,16 +1691,16 @@
       <c r="N48" s="1"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="6"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="2"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1735,14 +1713,14 @@
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="6"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="7"/>
+      <c r="F50" s="2"/>
       <c r="G50" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1755,7 +1733,7 @@
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="6"/>
@@ -1774,12 +1752,16 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
+      <c r="B52" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C52" s="3"/>
       <c r="D52" s="6"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
@@ -1789,17 +1771,13 @@
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="6"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -1809,10 +1787,10 @@
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="6"/>
       <c r="E54" s="1"/>
@@ -1831,7 +1809,7 @@
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="6"/>
@@ -1851,7 +1829,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="6"/>
@@ -1870,12 +1848,16 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="6"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -1885,19 +1867,15 @@
       <c r="N57" s="1"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="6"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -1905,15 +1883,19 @@
       <c r="N58" s="1"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
+      <c r="A59" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="6"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -1921,17 +1903,13 @@
       <c r="N59" s="1"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="6"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
@@ -1941,10 +1919,10 @@
       <c r="N60" s="1"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="A61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="6"/>
       <c r="E61" s="1"/>
@@ -1963,7 +1941,7 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="6"/>
@@ -1982,12 +1960,16 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
+      <c r="B63" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C63" s="3"/>
       <c r="D63" s="6"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -1997,16 +1979,12 @@
       <c r="N63" s="1"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="6"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -2017,10 +1995,10 @@
       <c r="N64" s="1"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="6"/>
       <c r="E65" s="2"/>
@@ -2039,7 +2017,7 @@
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="6"/>
@@ -2058,11 +2036,15 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
+      <c r="B67" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C67" s="3"/>
       <c r="D67" s="6"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -2073,17 +2055,13 @@
       <c r="N67" s="1"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="6"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -2093,13 +2071,17 @@
       <c r="N68" s="1"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
+      <c r="A69" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="6"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="9"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -2109,19 +2091,15 @@
       <c r="N69" s="1"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="6"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G70" s="9"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -2129,34 +2107,34 @@
       <c r="N70" s="1"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
+      <c r="A71" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="6"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A72" s="8" t="s">
-        <v>40</v>
-      </c>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="6"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
@@ -2164,15 +2142,19 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
+    <row r="73" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A73" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="6"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -2181,18 +2163,14 @@
       <c r="N73" s="1"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="6"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -2201,10 +2179,10 @@
       <c r="N74" s="1"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A75" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="6"/>
       <c r="E75" s="1"/>
@@ -2223,7 +2201,7 @@
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="6"/>
@@ -2242,13 +2220,17 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
+      <c r="B77" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C77" s="3"/>
       <c r="D77" s="6"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -2257,18 +2239,14 @@
       <c r="N77" s="1"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="6"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
@@ -2277,10 +2255,10 @@
       <c r="N78" s="1"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="A79" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="6"/>
       <c r="E79" s="1"/>
@@ -2298,13 +2276,17 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+      <c r="B80" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="C80" s="3"/>
       <c r="D80" s="6"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -2312,18 +2294,14 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
-        <v>46</v>
-      </c>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="6"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2332,14 +2310,18 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
+    <row r="82" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A82" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="6"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2349,17 +2331,13 @@
       <c r="N82" s="1"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="6"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -2370,16 +2348,16 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="6"/>
       <c r="E84" s="2"/>
-      <c r="F84" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G84" s="1"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
@@ -2389,12 +2367,16 @@
       <c r="N84" s="1"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
+      <c r="A85" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -2404,36 +2386,36 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
-        <v>70</v>
-      </c>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="6"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
+    <row r="87" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A87" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="6"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
@@ -2441,19 +2423,15 @@
       <c r="N87" s="1"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="6"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -2462,7 +2440,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -2482,7 +2460,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -2501,92 +2479,92 @@
       <c r="N90" s="1"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
+      <c r="A91" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="6"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
     </row>
-    <row r="92" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A92" s="8" t="s">
-        <v>71</v>
-      </c>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="6"/>
-      <c r="E92" s="2"/>
+      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="7"/>
-      <c r="I92" s="7"/>
-      <c r="J92" s="7"/>
-      <c r="K92" s="7"/>
-      <c r="L92" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
+    <row r="93" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A93" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="6"/>
-      <c r="E93" s="1"/>
+      <c r="E93" s="2"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+      <c r="L93" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="6"/>
-      <c r="E94" s="2"/>
+      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="A95" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="6"/>
       <c r="E95" s="2"/>
-      <c r="F95" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
@@ -2595,7 +2573,7 @@
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="6"/>
@@ -2615,18 +2593,18 @@
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="6"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G97" s="1"/>
-      <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-      <c r="J97" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -2635,7 +2613,7 @@
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="6"/>
@@ -2655,7 +2633,7 @@
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="6"/>
@@ -2675,7 +2653,7 @@
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="6"/>
@@ -2694,43 +2672,43 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
+      <c r="B101" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="C101" s="3"/>
       <c r="D101" s="6"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="6"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
-      <c r="J102" s="7"/>
-      <c r="K102" s="7"/>
-      <c r="L102" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2747,6 +2725,26 @@
       </c>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Senaste planeringen f�r Grafik
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering.xlsx
+++ b/Grafik/Planering/Grafikplanering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
   <si>
     <t>Vecka:</t>
   </si>
@@ -219,12 +219,6 @@
   </si>
   <si>
     <t>1.4.3 Siluett (Hela &amp; separata)</t>
-  </si>
-  <si>
-    <t>4.2 Text</t>
-  </si>
-  <si>
-    <t>4.2.1 Dialoger</t>
   </si>
   <si>
     <t>6 Text</t>
@@ -733,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O104"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +749,10 @@
       <c r="E1" s="3">
         <v>1</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>2</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="4">
         <v>3</v>
       </c>
       <c r="H1" s="3">
@@ -794,7 +788,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="6"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -831,11 +825,11 @@
       <c r="C4" s="3"/>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1236,10 +1230,10 @@
       <c r="C25" s="3"/>
       <c r="D25" s="6"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1272,10 +1266,10 @@
       <c r="C27" s="3"/>
       <c r="D27" s="6"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1292,10 +1286,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="6"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1312,10 +1306,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="6"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1372,7 +1366,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1539,7 +1533,7 @@
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="6"/>
@@ -1559,7 +1553,7 @@
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="6"/>
@@ -1662,7 +1656,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="6"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="7"/>
+      <c r="F47" s="2"/>
       <c r="G47" s="1"/>
       <c r="H47" s="7"/>
       <c r="I47" s="9" t="s">
@@ -1698,9 +1692,9 @@
       <c r="C49" s="3"/>
       <c r="D49" s="6"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="7"/>
+      <c r="F49" s="2"/>
       <c r="G49" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1738,9 +1732,9 @@
       <c r="C51" s="3"/>
       <c r="D51" s="6"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="7"/>
+      <c r="F51" s="2"/>
       <c r="G51" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -1758,9 +1752,9 @@
       <c r="C52" s="3"/>
       <c r="D52" s="6"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="7"/>
+      <c r="F52" s="2"/>
       <c r="G52" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -2151,9 +2145,9 @@
       <c r="D73" s="6"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="7"/>
+      <c r="G73" s="2"/>
       <c r="H73" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -2187,9 +2181,9 @@
       <c r="D75" s="6"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="7"/>
+      <c r="G75" s="2"/>
       <c r="H75" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
@@ -2207,9 +2201,9 @@
       <c r="D76" s="6"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="7"/>
+      <c r="G76" s="2"/>
       <c r="H76" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
@@ -2227,9 +2221,9 @@
       <c r="D77" s="6"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="7"/>
+      <c r="G77" s="2"/>
       <c r="H77" s="9" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
@@ -2254,19 +2248,19 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>68</v>
+    <row r="79" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A79" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="6"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -2276,17 +2270,13 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
-      <c r="B80" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="6"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -2295,13 +2285,17 @@
       <c r="N80" s="1"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
+      <c r="A81" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="6"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
@@ -2310,18 +2304,18 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A82" s="8" t="s">
-        <v>46</v>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="6"/>
       <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="F82" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
@@ -2346,20 +2340,20 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>44</v>
+    <row r="84" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A84" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="6"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
@@ -2367,16 +2361,12 @@
       <c r="N84" s="1"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -2387,24 +2377,28 @@
       <c r="N85" s="1"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
+      <c r="A86" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="6"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
     </row>
-    <row r="87" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A87" s="8" t="s">
-        <v>70</v>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -2423,15 +2417,19 @@
       <c r="N87" s="1"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
+      <c r="A88" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="6"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -2439,59 +2437,51 @@
       <c r="N88" s="1"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="6"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>84</v>
+    <row r="90" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A90" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="1"/>
+      <c r="E90" s="2"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="7"/>
+      <c r="G90" s="1"/>
       <c r="H90" s="7"/>
-      <c r="I90" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="6"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
@@ -2499,48 +2489,56 @@
       <c r="N91" s="1"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
+      <c r="A92" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="6"/>
-      <c r="E92" s="1"/>
+      <c r="E92" s="2"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A93" s="8" t="s">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="6"/>
       <c r="E93" s="2"/>
-      <c r="F93" s="1"/>
+      <c r="F93" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G93" s="1"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
+      <c r="B94" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="C94" s="3"/>
       <c r="D94" s="6"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -2551,19 +2549,19 @@
       <c r="N94" s="1"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B95" s="3"/>
+      <c r="A95" s="3"/>
+      <c r="B95" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="C95" s="3"/>
       <c r="D95" s="6"/>
-      <c r="E95" s="2"/>
+      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="9" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
@@ -2573,18 +2571,18 @@
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="6"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
       <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
@@ -2593,18 +2591,18 @@
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="6"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
       <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -2613,7 +2611,7 @@
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="6"/>
@@ -2632,29 +2630,25 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
-      <c r="B99" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="6"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3" t="s">
+      <c r="A100" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="6"/>
       <c r="E100" s="1"/>
@@ -2662,19 +2656,19 @@
       <c r="G100" s="1"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
-      <c r="J100" s="9" t="s">
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+      <c r="L100" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3" t="s">
+      <c r="A101" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="6"/>
       <c r="E101" s="1"/>
@@ -2682,69 +2676,13 @@
       <c r="G101" s="1"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
-      <c r="J101" s="9" t="s">
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="7"/>
-      <c r="I103" s="7"/>
-      <c r="J103" s="7"/>
-      <c r="K103" s="7"/>
-      <c r="L103" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="7"/>
-      <c r="I104" s="7"/>
-      <c r="J104" s="7"/>
-      <c r="K104" s="7"/>
-      <c r="L104" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uppdatering av planering och huvudmenyn
</commit_message>
<xml_diff>
--- a/Grafik/Planering/Grafikplanering.xlsx
+++ b/Grafik/Planering/Grafikplanering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
   <si>
     <t>Vecka:</t>
   </si>
@@ -254,9 +254,6 @@
     <t>3.1.9 Trappräcke</t>
   </si>
   <si>
-    <t>6.3 Menybakgrund</t>
-  </si>
-  <si>
     <t>73% Färdigt</t>
   </si>
   <si>
@@ -341,7 +338,7 @@
     <t>6.2 Huvudmeny</t>
   </si>
   <si>
-    <t>30% Färdigt</t>
+    <t>70% Färdigt</t>
   </si>
 </sst>
 </file>
@@ -854,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O118"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+      <selection activeCell="S93" sqref="S93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +955,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="7"/>
       <c r="H4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1495,7 +1492,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="7"/>
       <c r="H32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1748,7 +1745,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="6"/>
       <c r="E45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="9" t="s">
@@ -2528,7 +2525,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -2538,7 +2535,7 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -2548,7 +2545,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -2567,92 +2564,92 @@
       <c r="N88" s="1"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="6"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
+    <row r="90" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A90" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="1"/>
+      <c r="E90" s="2"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
     </row>
-    <row r="91" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A91" s="8" t="s">
-        <v>66</v>
-      </c>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="6"/>
-      <c r="E91" s="2"/>
+      <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="7"/>
-      <c r="J91" s="7"/>
-      <c r="K91" s="7"/>
-      <c r="L91" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
+      <c r="A92" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="6"/>
-      <c r="E92" s="1"/>
+      <c r="E92" s="2"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B93" s="3"/>
+      <c r="A93" s="3"/>
+      <c r="B93" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="C93" s="3"/>
       <c r="D93" s="6"/>
       <c r="E93" s="2"/>
-      <c r="F93" s="1"/>
+      <c r="F93" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="G93" s="1"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
@@ -2661,7 +2658,7 @@
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="6"/>
@@ -2681,18 +2678,18 @@
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="6"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
+      <c r="H95" s="7"/>
+      <c r="I95" s="7"/>
+      <c r="J95" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
@@ -2701,7 +2698,7 @@
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="6"/>
@@ -2718,10 +2715,10 @@
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="6"/>
@@ -2738,10 +2735,10 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="6"/>
@@ -2758,45 +2755,45 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
-      <c r="B99" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="6"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="6"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+      <c r="L100" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -2814,83 +2811,83 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>75</v>
-      </c>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="6"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
-      <c r="J102" s="7"/>
-      <c r="K102" s="7"/>
-      <c r="L102" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A103" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="6"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
     </row>
-    <row r="104" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A104" s="8" t="s">
-        <v>83</v>
-      </c>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="6"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="7"/>
-      <c r="I104" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="6"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="6"/>
       <c r="E106" s="1"/>
@@ -2906,7 +2903,7 @@
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3" t="s">
         <v>85</v>
@@ -2926,7 +2923,7 @@
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3" t="s">
         <v>86</v>
@@ -2946,166 +2943,166 @@
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
-      <c r="B109" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="6"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="7"/>
-      <c r="H109" s="7"/>
-      <c r="I109" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A110" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="6"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
-      <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-    </row>
-    <row r="111" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A111" s="8" t="s">
+      <c r="G110" s="12" t="s">
         <v>88</v>
       </c>
+      <c r="H110" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I110" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J110" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K110" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="L110" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M110" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="N110" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="6"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="12" t="s">
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+    </row>
+    <row r="112" spans="1:15" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H111" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="I111" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J111" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="K111" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L111" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M111" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="N111" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="6"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="1"/>
-      <c r="L112" s="1"/>
-      <c r="M112" s="1"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+      <c r="I112" s="12"/>
+      <c r="J112" s="12"/>
+      <c r="K112" s="12"/>
+      <c r="L112" s="12"/>
+      <c r="M112" s="12"/>
       <c r="N112" s="1"/>
-    </row>
-    <row r="113" spans="1:15" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="O112" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="6"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
-      <c r="G113" s="12"/>
-      <c r="H113" s="12"/>
-      <c r="I113" s="12"/>
-      <c r="J113" s="12"/>
-      <c r="K113" s="12"/>
-      <c r="L113" s="12"/>
-      <c r="M113" s="12"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="6"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
+      <c r="G114" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
+      <c r="I114" s="9"/>
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
-      <c r="M114" s="1"/>
+      <c r="M114" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="N114" s="1"/>
-      <c r="O114" s="13" t="s">
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="6"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
-      <c r="G115" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H115" s="1"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="14">
+        <v>41335</v>
+      </c>
       <c r="I115" s="9"/>
       <c r="J115" s="1"/>
-      <c r="K115" s="1"/>
+      <c r="K115" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="L115" s="1"/>
-      <c r="M115" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="M115" s="1"/>
       <c r="N115" s="1"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="6"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="9"/>
-      <c r="H116" s="14">
-        <v>41335</v>
+      <c r="H116" s="15" t="s">
+        <v>98</v>
       </c>
       <c r="I116" s="9"/>
       <c r="J116" s="1"/>
@@ -3123,9 +3120,9 @@
       <c r="D117" s="6"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="9"/>
+      <c r="G117" s="1"/>
       <c r="H117" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I117" s="9"/>
       <c r="J117" s="1"/>
@@ -3135,26 +3132,6 @@
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I118" s="9"/>
-      <c r="J118" s="1"/>
-      <c r="K118" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="L118" s="1"/>
-      <c r="M118" s="1"/>
-      <c r="N118" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>